<commit_message>
Added graphs from TSL
</commit_message>
<xml_diff>
--- a/Useful data_files/TSL/tsl-dosimetry-may2014.xlsx
+++ b/Useful data_files/TSL/tsl-dosimetry-may2014.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2000" windowWidth="21880" windowHeight="12500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="1995" windowWidth="21885" windowHeight="12495" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminary results" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="190">
   <si>
     <t>PLL</t>
   </si>
@@ -573,16 +573,35 @@
   </si>
   <si>
     <t>RCU Trigger with lower resistor value</t>
+  </si>
+  <si>
+    <t>(MeVcm2/g)</t>
+  </si>
+  <si>
+    <t>1kRad</t>
+  </si>
+  <si>
+    <t>J/g</t>
+  </si>
+  <si>
+    <t>PLL1</t>
+  </si>
+  <si>
+    <t>PLL2</t>
+  </si>
+  <si>
+    <t>PLL3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1090,7 +1109,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1100,15 +1119,16 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="433">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1871,36 +1891,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:U71"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13.5" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="18.375" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="15"/>
       <c r="I1" t="s">
         <v>99</v>
       </c>
@@ -1969,11 +1989,11 @@
         <v>19.559999999999999</v>
       </c>
       <c r="E3" s="2">
-        <f>D3/$D$3</f>
+        <f t="shared" ref="E3:E9" si="0">D3/$D$3</f>
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <f>D3*2.33/10</f>
+        <f t="shared" ref="F3:F9" si="1">D3*2.33/10</f>
         <v>4.55748</v>
       </c>
       <c r="G3" s="1">
@@ -1981,11 +2001,11 @@
         <v>2.9400000000000002E-10</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H9" si="0">G3*100</f>
+        <f t="shared" ref="H3:H9" si="2">G3*100</f>
         <v>2.9400000000000002E-8</v>
       </c>
       <c r="I3" s="1">
-        <f>1.602E-19*1000000*D3*100/(1000*0.000001)</f>
+        <f t="shared" ref="I3:I9" si="3">1.602E-19*1000000*D3*100/(1000*0.000001)</f>
         <v>3.133512E-7</v>
       </c>
       <c r="J3" s="1">
@@ -1999,36 +2019,36 @@
         <v>1</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M8" si="1">J3*$C$13</f>
+        <f t="shared" ref="M3:M8" si="4">J3*$C$13</f>
         <v>2.375E-2</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N8" si="2">1/(M3*L3)</f>
+        <f t="shared" ref="N3:N8" si="5">1/(M3*L3)</f>
         <v>42.10526315789474</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <f t="shared" ref="P3:P8" si="3">J3*$C$14</f>
+        <f t="shared" ref="P3:P8" si="6">J3*$C$14</f>
         <v>1.5199999999999998E-4</v>
       </c>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q8" si="4">1/(P3*L3)</f>
+        <f t="shared" ref="Q3:Q8" si="7">1/(P3*L3)</f>
         <v>6578.9473684210534</v>
       </c>
       <c r="R3" s="2">
-        <f>$C$13*I3*60/1000</f>
+        <f t="shared" ref="R3:R9" si="8">$C$13*I3*60/1000</f>
         <v>4.7002680000000003</v>
       </c>
       <c r="S3" s="2">
-        <f t="shared" ref="S3:S9" si="5">R3*60</f>
+        <f t="shared" ref="S3:S9" si="9">R3*60</f>
         <v>282.01608000000004</v>
       </c>
       <c r="T3" s="1">
-        <f>$C$14*I3*60/1000</f>
+        <f t="shared" ref="T3:T9" si="10">$C$14*I3*60/1000</f>
         <v>3.0081715200000001E-2</v>
       </c>
       <c r="U3" s="2">
-        <f t="shared" ref="U3:U9" si="6">T3*60</f>
+        <f t="shared" ref="U3:U9" si="11">T3*60</f>
         <v>1.804902912</v>
       </c>
     </row>
@@ -2043,23 +2063,23 @@
         <v>3.4319999999999999</v>
       </c>
       <c r="E4" s="2">
-        <f>D4/$D$3</f>
+        <f t="shared" si="0"/>
         <v>0.17546012269938652</v>
       </c>
       <c r="F4" s="2">
-        <f>D4*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>0.79965599999999992</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G9" si="7">$G$3*E4</f>
+        <f t="shared" ref="G4:G9" si="12">$G$3*E4</f>
         <v>5.1585276073619637E-11</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.1585276073619637E-9</v>
       </c>
       <c r="I4" s="1">
-        <f>1.602E-19*1000000*D4*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>5.4980639999999999E-8</v>
       </c>
       <c r="J4" s="1">
@@ -2072,36 +2092,36 @@
         <v>1</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3124.9999999999995</v>
       </c>
       <c r="R4" s="2">
-        <f>$C$13*I4*60/1000</f>
+        <f t="shared" si="8"/>
         <v>0.82470960000000004</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>49.482576000000002</v>
       </c>
       <c r="T4" s="1">
-        <f>$C$14*I4*60/1000</f>
+        <f t="shared" si="10"/>
         <v>5.2781414400000001E-3</v>
       </c>
       <c r="U4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.31668848640000002</v>
       </c>
     </row>
@@ -2116,23 +2136,23 @@
         <v>12.95</v>
       </c>
       <c r="E5" s="2">
-        <f>D5/$D$3</f>
+        <f t="shared" si="0"/>
         <v>0.66206543967280163</v>
       </c>
       <c r="F5" s="2">
-        <f>D5*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>3.01735</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.946472392638037E-10</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.946472392638037E-8</v>
       </c>
       <c r="I5" s="1">
-        <f>1.602E-19*1000000*D5*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>2.0745899999999995E-7</v>
       </c>
       <c r="J5" s="1">
@@ -2145,36 +2165,36 @@
         <v>2000</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.7499999999999997E-6</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>133.33333333333334</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4E-8</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>20833.333333333332</v>
       </c>
       <c r="R5" s="2">
-        <f>$C$13*I5*60/1000</f>
+        <f t="shared" si="8"/>
         <v>3.1118849999999991</v>
       </c>
       <c r="S5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>186.71309999999994</v>
       </c>
       <c r="T5" s="1">
-        <f>$C$14*I5*60/1000</f>
+        <f t="shared" si="10"/>
         <v>1.9916063999999994E-2</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1949638399999996</v>
       </c>
     </row>
@@ -2189,23 +2209,23 @@
         <v>16.059999999999999</v>
       </c>
       <c r="E6" s="2">
-        <f>D6/$D$3</f>
+        <f t="shared" si="0"/>
         <v>0.82106339468302658</v>
       </c>
       <c r="F6" s="2">
-        <f>D6*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>3.7419799999999994</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.4139263803680981E-10</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.413926380368098E-8</v>
       </c>
       <c r="I6" s="1">
-        <f>1.602E-19*1000000*D6*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>2.572812E-7</v>
       </c>
       <c r="J6" s="1">
@@ -2218,36 +2238,36 @@
         <v>2000</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.05E-6</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>163.93442622950818</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.9519999999999999E-8</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>25614.754098360656</v>
       </c>
       <c r="R6" s="2">
-        <f>$C$13*I6*60/1000</f>
+        <f t="shared" si="8"/>
         <v>3.8592180000000003</v>
       </c>
       <c r="S6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>231.55308000000002</v>
       </c>
       <c r="T6" s="1">
-        <f>$C$14*I6*60/1000</f>
+        <f t="shared" si="10"/>
         <v>2.4698995199999997E-2</v>
       </c>
       <c r="U6" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.4819397119999997</v>
       </c>
     </row>
@@ -2262,23 +2282,23 @@
         <v>19.559999999999999</v>
       </c>
       <c r="E7" s="2">
-        <f>D7/$D$3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <f>D7*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>4.55748</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.9400000000000002E-10</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.9400000000000002E-8</v>
       </c>
       <c r="I7" s="1">
-        <f>1.602E-19*1000000*D7*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>3.133512E-7</v>
       </c>
       <c r="J7" s="1">
@@ -2292,36 +2312,36 @@
         <v>65536</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.7499999999999999E-6</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.5486505681818183</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.7600000000000002E-8</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>866.97665127840901</v>
       </c>
       <c r="R7" s="2">
-        <f>$C$13*I7*60/1000</f>
+        <f t="shared" si="8"/>
         <v>4.7002680000000003</v>
       </c>
       <c r="S7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>282.01608000000004</v>
       </c>
       <c r="T7" s="1">
-        <f>$C$14*I7*60/1000</f>
+        <f t="shared" si="10"/>
         <v>3.0081715200000001E-2</v>
       </c>
       <c r="U7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.804902912</v>
       </c>
     </row>
@@ -2336,23 +2356,23 @@
         <v>19.559999999999999</v>
       </c>
       <c r="E8" s="2">
-        <f>D8/$D$3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <f>D8*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>4.55748</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.9400000000000002E-10</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.9400000000000002E-8</v>
       </c>
       <c r="I8" s="1">
-        <f>1.602E-19*1000000*D8*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>3.133512E-7</v>
       </c>
       <c r="J8" s="1">
@@ -2366,36 +2386,36 @@
         <v>1114112</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.17951516544117646</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2000000000000002E-8</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>28.049244600183822</v>
       </c>
       <c r="R8" s="2">
-        <f>$C$13*I8*60/1000</f>
+        <f t="shared" si="8"/>
         <v>4.7002680000000003</v>
       </c>
       <c r="S8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>282.01608000000004</v>
       </c>
       <c r="T8" s="1">
-        <f>$C$14*I8*60/1000</f>
+        <f t="shared" si="10"/>
         <v>3.0081715200000001E-2</v>
       </c>
       <c r="U8" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.804902912</v>
       </c>
     </row>
@@ -2410,39 +2430,39 @@
         <v>4.0069999999999997</v>
       </c>
       <c r="E9" s="2">
-        <f>D9/$D$3</f>
+        <f t="shared" si="0"/>
         <v>0.20485685071574641</v>
       </c>
       <c r="F9" s="2">
-        <f>D9*2.33/10</f>
+        <f t="shared" si="1"/>
         <v>0.93363099999999988</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.0227914110429445E-11</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0227914110429448E-9</v>
       </c>
       <c r="I9" s="1">
-        <f>1.602E-19*1000000*D9*100/(1000*0.000001)</f>
+        <f t="shared" si="3"/>
         <v>6.4192139999999975E-8</v>
       </c>
       <c r="R9" s="2">
-        <f>$C$13*I9*60/1000</f>
+        <f t="shared" si="8"/>
         <v>0.96288209999999974</v>
       </c>
       <c r="S9" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>57.772925999999984</v>
       </c>
       <c r="T9" s="1">
-        <f>$C$14*I9*60/1000</f>
+        <f t="shared" si="10"/>
         <v>6.1624454399999981E-3</v>
       </c>
       <c r="U9" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.36974672639999989</v>
       </c>
     </row>
@@ -2936,35 +2956,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="14" customWidth="1"/>
+    <col min="9" max="9" width="14" style="13" customWidth="1"/>
     <col min="10" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="14" style="14" customWidth="1"/>
-    <col min="13" max="13" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="29.1640625" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="13" customWidth="1"/>
+    <col min="13" max="13" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.125" customWidth="1"/>
+    <col min="15" max="17" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.125" customWidth="1"/>
+    <col min="19" max="19" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:20">
       <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="I1" s="12"/>
+      <c r="L1" s="12"/>
       <c r="N1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="O1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2989,7 +3020,7 @@
       <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>60</v>
       </c>
       <c r="J2" t="s">
@@ -2998,20 +3029,20 @@
       <c r="K2" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>62</v>
       </c>
       <c r="M2" t="s">
         <v>71</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>113</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>20140507</v>
       </c>
@@ -3028,7 +3059,7 @@
         <v>134000</v>
       </c>
       <c r="F3">
-        <f>E3/100</f>
+        <f t="shared" ref="F3:F10" si="0">E3/100</f>
         <v>1340</v>
       </c>
       <c r="G3">
@@ -3037,20 +3068,21 @@
       <c r="H3" s="1">
         <v>78500</v>
       </c>
-      <c r="I3" s="13">
-        <f>H3*D3</f>
+      <c r="I3" s="12">
+        <f t="shared" ref="I3:I10" si="1">H3*D3</f>
         <v>2781333500</v>
       </c>
       <c r="J3" s="1">
-        <f>I3/F3</f>
+        <f t="shared" ref="J3:J10" si="2">I3/F3</f>
         <v>2075622.014925373</v>
       </c>
       <c r="K3" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L3" s="15">
-        <f>K3*I3/1000</f>
-        <v>0.16688001</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L3" s="14">
+        <f t="shared" ref="L3:L10" si="3">K3*I3/1000</f>
+        <v>0.1733265847863</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>72</v>
@@ -3058,11 +3090,14 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>20140507</v>
       </c>
@@ -3079,7 +3114,7 @@
         <v>14235</v>
       </c>
       <c r="F4" s="4">
-        <f>E4/100</f>
+        <f t="shared" si="0"/>
         <v>142.35</v>
       </c>
       <c r="G4">
@@ -3088,20 +3123,21 @@
       <c r="H4" s="1">
         <v>78500</v>
       </c>
-      <c r="I4" s="13">
-        <f>H4*D4</f>
+      <c r="I4" s="12">
+        <f t="shared" si="1"/>
         <v>13930060500</v>
       </c>
       <c r="J4" s="1">
-        <f>I4/F4</f>
+        <f t="shared" si="2"/>
         <v>97857818.756585881</v>
       </c>
       <c r="K4" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L4" s="15">
-        <f>K4*I4/1000</f>
-        <v>0.83580362999999991</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="3"/>
+        <v>0.86809072422690003</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>73</v>
@@ -3109,11 +3145,14 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" t="s">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>20140507</v>
       </c>
@@ -3130,7 +3169,7 @@
         <v>16000</v>
       </c>
       <c r="F5" s="4">
-        <f>E5/100</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="G5">
@@ -3139,31 +3178,35 @@
       <c r="H5" s="1">
         <v>78500</v>
       </c>
-      <c r="I5" s="13">
-        <f>H5*D5</f>
+      <c r="I5" s="12">
+        <f t="shared" si="1"/>
         <v>19831690500</v>
       </c>
       <c r="J5" s="1">
-        <f>I5/F5</f>
+        <f t="shared" si="2"/>
         <v>123948065.625</v>
       </c>
       <c r="K5" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L5" s="15">
-        <f>K5*I5/1000</f>
-        <v>1.1899014299999999</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="3"/>
+        <v>1.2358673222409002</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>74</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" t="s">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>20140507</v>
       </c>
@@ -3180,7 +3223,7 @@
         <v>83854</v>
       </c>
       <c r="F6" s="4">
-        <f>E6/100</f>
+        <f t="shared" si="0"/>
         <v>838.54</v>
       </c>
       <c r="G6">
@@ -3189,32 +3232,33 @@
       <c r="H6" s="1">
         <v>78500</v>
       </c>
-      <c r="I6" s="13">
-        <f>H6*D6</f>
+      <c r="I6" s="12">
+        <f t="shared" si="1"/>
         <v>106483130500</v>
       </c>
       <c r="J6" s="1">
-        <f>I6/F6</f>
+        <f t="shared" si="2"/>
         <v>126986345.91074964</v>
       </c>
       <c r="K6" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L6" s="15">
-        <f>K6*I6/1000</f>
-        <v>6.3889878299999987</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="3"/>
+        <v>6.6357944298729006</v>
       </c>
       <c r="M6" t="s">
         <v>76</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>20140507</v>
       </c>
@@ -3231,7 +3275,7 @@
         <v>21260</v>
       </c>
       <c r="F7" s="4">
-        <f>E7/100</f>
+        <f t="shared" si="0"/>
         <v>212.6</v>
       </c>
       <c r="G7">
@@ -3240,29 +3284,30 @@
       <c r="H7" s="1">
         <v>78500</v>
       </c>
-      <c r="I7" s="13">
-        <f>H7*D7</f>
+      <c r="I7" s="12">
+        <f t="shared" si="1"/>
         <v>26569424000</v>
       </c>
       <c r="J7" s="1">
-        <f>I7/F7</f>
+        <f t="shared" si="2"/>
         <v>124973772.34242709</v>
       </c>
       <c r="K7" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L7" s="15">
-        <f>K7*I7/1000</f>
-        <v>1.5941654399999998</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="3"/>
+        <v>1.6557480509472002</v>
       </c>
       <c r="M7" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>20140507</v>
       </c>
@@ -3279,7 +3324,7 @@
         <v>53453</v>
       </c>
       <c r="F8" s="4">
-        <f>E8/100</f>
+        <f t="shared" si="0"/>
         <v>534.53</v>
       </c>
       <c r="G8">
@@ -3288,29 +3333,30 @@
       <c r="H8" s="1">
         <v>78500</v>
       </c>
-      <c r="I8" s="13">
-        <f>H8*D8</f>
+      <c r="I8" s="12">
+        <f t="shared" si="1"/>
         <v>67351194500</v>
       </c>
       <c r="J8" s="1">
-        <f>I8/F8</f>
+        <f t="shared" si="2"/>
         <v>126000775.44758947</v>
       </c>
       <c r="K8" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L8" s="15">
-        <f>K8*I8/1000</f>
-        <v>4.04107167</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="3"/>
+        <v>4.1971782686121006</v>
       </c>
       <c r="M8" t="s">
         <v>80</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="T8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>20140507</v>
       </c>
@@ -3327,7 +3373,7 @@
         <v>63151</v>
       </c>
       <c r="F9" s="4">
-        <f>E9/100</f>
+        <f t="shared" si="0"/>
         <v>631.51</v>
       </c>
       <c r="G9">
@@ -3336,32 +3382,33 @@
       <c r="H9" s="1">
         <v>78500</v>
       </c>
-      <c r="I9" s="13">
-        <f>H9*D9</f>
+      <c r="I9" s="12">
+        <f t="shared" si="1"/>
         <v>80699177500</v>
       </c>
       <c r="J9" s="1">
-        <f>I9/F9</f>
+        <f t="shared" si="2"/>
         <v>127787647.85989137</v>
       </c>
       <c r="K9" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L9" s="15">
-        <f>K9*I9/1000</f>
-        <v>4.8419506499999994</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="3"/>
+        <v>5.0289952036095</v>
       </c>
       <c r="M9" t="s">
         <v>84</v>
       </c>
-      <c r="P9" t="s">
+      <c r="S9" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="T9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>20140507</v>
       </c>
@@ -3378,7 +3425,7 @@
         <v>277505</v>
       </c>
       <c r="F10" s="4">
-        <f>E10/100</f>
+        <f t="shared" si="0"/>
         <v>2775.05</v>
       </c>
       <c r="G10">
@@ -3387,32 +3434,39 @@
       <c r="H10" s="1">
         <v>78500</v>
       </c>
-      <c r="I10" s="13">
-        <f>H10*D10</f>
+      <c r="I10" s="12">
+        <f t="shared" si="1"/>
         <v>360091353500</v>
       </c>
       <c r="J10" s="1">
-        <f>I10/F10</f>
+        <f t="shared" si="2"/>
         <v>129760311.88627231</v>
       </c>
       <c r="K10" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L10" s="15">
-        <f>K10*I10/1000</f>
-        <v>21.605481209999997</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="3"/>
+        <v>22.440100949142302</v>
       </c>
       <c r="M10" t="s">
         <v>88</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>87</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="T10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="11" spans="1:20">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>20140508</v>
       </c>
@@ -3438,32 +3492,33 @@
       <c r="H13" s="1">
         <v>78500</v>
       </c>
-      <c r="I13" s="13">
-        <f>H13*D13</f>
+      <c r="I13" s="12">
+        <f t="shared" ref="I13:I20" si="4">H13*D13</f>
         <v>1149318500</v>
       </c>
       <c r="J13" s="1">
-        <f>I13/F13</f>
+        <f t="shared" ref="J13:J20" si="5">I13/F13</f>
         <v>22072565.776838869</v>
       </c>
       <c r="K13" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L13" s="15">
-        <f>K13*I13/1000</f>
-        <v>6.895910999999999E-2</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" ref="L13:L20" si="6">K13*I13/1000</f>
+        <v>7.1623000419300017E-2</v>
       </c>
       <c r="M13" t="s">
         <v>110</v>
       </c>
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>115</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="T13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>20140508</v>
       </c>
@@ -3489,32 +3544,33 @@
       <c r="H14" s="1">
         <v>78500</v>
       </c>
-      <c r="I14" s="13">
-        <f>H14*D14</f>
+      <c r="I14" s="12">
+        <f t="shared" si="4"/>
         <v>1551788000</v>
       </c>
       <c r="J14" s="1">
-        <f>I14/F14</f>
+        <f t="shared" si="5"/>
         <v>21072623.574144486</v>
       </c>
       <c r="K14" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L14" s="15">
-        <f>K14*I14/1000</f>
-        <v>9.3107279999999987E-2</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="6"/>
+        <v>9.6704014226400001E-2</v>
       </c>
       <c r="M14" t="s">
         <v>111</v>
       </c>
-      <c r="P14" t="s">
+      <c r="S14" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="T14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>20140508</v>
       </c>
@@ -3540,20 +3596,21 @@
       <c r="H15" s="1">
         <v>78500</v>
       </c>
-      <c r="I15" s="13">
-        <f>H15*D15</f>
+      <c r="I15" s="12">
+        <f t="shared" si="4"/>
         <v>48803685500</v>
       </c>
       <c r="J15" s="1">
-        <f>I15/F15</f>
+        <f t="shared" si="5"/>
         <v>26573712.252387643</v>
       </c>
       <c r="K15" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L15" s="15">
-        <f>K15*I15/1000</f>
-        <v>2.9282211299999998</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="6"/>
+        <v>3.0413383122519004</v>
       </c>
       <c r="M15" t="s">
         <v>112</v>
@@ -3561,18 +3618,18 @@
       <c r="N15">
         <v>42</v>
       </c>
-      <c r="O15" s="1">
+      <c r="R15" s="1">
         <f>N15/(I15+I14)</f>
         <v>8.3407020291448554E-10</v>
       </c>
-      <c r="P15" t="s">
+      <c r="S15" t="s">
         <v>115</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="T15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>20140508</v>
       </c>
@@ -3585,26 +3642,27 @@
       <c r="H16" s="1">
         <v>78500</v>
       </c>
-      <c r="I16" s="13">
-        <f>H16*D16</f>
+      <c r="I16" s="12">
+        <f t="shared" si="4"/>
         <v>4874928500</v>
       </c>
       <c r="J16" s="1" t="e">
-        <f>I16/F16</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L16" s="15">
-        <f>K16*I16/1000</f>
-        <v>0.29249570999999996</v>
-      </c>
-      <c r="Q16" t="s">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="6"/>
+        <v>0.30379481927730001</v>
+      </c>
+      <c r="T16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>20140508</v>
       </c>
@@ -3630,32 +3688,33 @@
       <c r="H17" s="1">
         <v>78500</v>
       </c>
-      <c r="I17" s="13">
-        <f>H17*D17</f>
+      <c r="I17" s="12">
+        <f t="shared" si="4"/>
         <v>3510520000</v>
       </c>
       <c r="J17" s="1">
-        <f>I17/F17</f>
+        <f t="shared" si="5"/>
         <v>23135099.512323711</v>
       </c>
       <c r="K17" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L17" s="15">
-        <f>K17*I17/1000</f>
-        <v>0.21063119999999999</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="6"/>
+        <v>0.218767883256</v>
       </c>
       <c r="M17" t="s">
         <v>119</v>
       </c>
-      <c r="P17" t="s">
+      <c r="S17" t="s">
         <v>115</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="T17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>20140508</v>
       </c>
@@ -3681,20 +3740,21 @@
       <c r="H18" s="1">
         <v>78500</v>
       </c>
-      <c r="I18" s="13">
-        <f>H18*D18</f>
+      <c r="I18" s="12">
+        <f t="shared" si="4"/>
         <v>49970038500</v>
       </c>
       <c r="J18" s="1">
-        <f>I18/F18</f>
+        <f t="shared" si="5"/>
         <v>26393787.666710682</v>
       </c>
       <c r="K18" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L18" s="15">
-        <f>K18*I18/1000</f>
-        <v>2.9982023099999995</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="6"/>
+        <v>3.1140228652353001</v>
       </c>
       <c r="M18" t="s">
         <v>119</v>
@@ -3702,18 +3762,18 @@
       <c r="N18">
         <v>28</v>
       </c>
-      <c r="O18" s="1">
+      <c r="R18" s="1">
         <f>N18/(I18+I17)</f>
         <v>5.235547418600724E-10</v>
       </c>
-      <c r="P18" t="s">
+      <c r="S18" t="s">
         <v>117</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="T18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>20140508</v>
       </c>
@@ -3739,20 +3799,21 @@
       <c r="H19" s="1">
         <v>78500</v>
       </c>
-      <c r="I19" s="13">
-        <f>H19*D19</f>
+      <c r="I19" s="12">
+        <f t="shared" si="4"/>
         <v>58763137500</v>
       </c>
       <c r="J19" s="1">
-        <f>I19/F19</f>
+        <f t="shared" si="5"/>
         <v>26621335.571290724</v>
       </c>
       <c r="K19" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L19" s="15">
-        <f>K19*I19/1000</f>
-        <v>3.5257882499999997</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="6"/>
+        <v>3.6619894500975003</v>
       </c>
       <c r="M19" t="s">
         <v>121</v>
@@ -3760,18 +3821,18 @@
       <c r="N19">
         <v>38</v>
       </c>
-      <c r="O19" s="1">
+      <c r="R19" s="1">
         <f>N19/I19</f>
         <v>6.4666390558196451E-10</v>
       </c>
-      <c r="P19" t="s">
+      <c r="S19" t="s">
         <v>120</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="T19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>20140508</v>
       </c>
@@ -3797,20 +3858,21 @@
       <c r="H20" s="1">
         <v>78500</v>
       </c>
-      <c r="I20" s="13">
-        <f>H20*D20</f>
+      <c r="I20" s="12">
+        <f t="shared" si="4"/>
         <v>23620885500</v>
       </c>
       <c r="J20" s="1">
-        <f>I20/F20</f>
+        <f t="shared" si="5"/>
         <v>24605089.0625</v>
       </c>
       <c r="K20" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L20" s="15">
-        <f>K20*I20/1000</f>
-        <v>1.4172531299999998</v>
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="6"/>
+        <v>1.4720016184119002</v>
       </c>
       <c r="M20" t="s">
         <v>124</v>
@@ -3818,24 +3880,25 @@
       <c r="N20">
         <v>20</v>
       </c>
-      <c r="O20" s="1">
+      <c r="R20" s="1">
         <f>N20/I20</f>
         <v>8.4670830820461832E-10</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
         <v>122</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="T20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:20">
       <c r="F21" s="4"/>
-      <c r="Q21" t="s">
+      <c r="K21" s="1"/>
+      <c r="T21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>20140508</v>
       </c>
@@ -3861,32 +3924,33 @@
       <c r="H22" s="1">
         <v>78500</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <f>H22*D22</f>
         <v>34998518500</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="10">
         <f>I22/F22</f>
         <v>18768779.495044831</v>
       </c>
       <c r="K22" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L22" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L22" s="14">
         <f>K22*I22/1000</f>
-        <v>2.0999111099999999</v>
+        <v>2.1810306761793004</v>
       </c>
       <c r="M22" t="s">
         <v>128</v>
       </c>
-      <c r="P22" t="s">
+      <c r="S22" t="s">
         <v>115</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="T22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>20140508</v>
       </c>
@@ -3912,30 +3976,31 @@
       <c r="H23" s="1">
         <v>78500</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="12">
         <f>H23*D23</f>
         <v>27376325500</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="11">
         <f>I23/F23</f>
         <v>26242391.752379674</v>
       </c>
       <c r="K23" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L23" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L23" s="14">
         <f>K23*I23/1000</f>
-        <v>1.6425795299999997</v>
+        <v>1.7060323772439001</v>
       </c>
       <c r="M23" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="1"/>
-      <c r="P23" t="s">
+      <c r="R23" s="1"/>
+      <c r="S23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>20140508</v>
       </c>
@@ -3961,47 +4026,56 @@
       <c r="H24" s="1">
         <v>78500</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <f>H24*D24</f>
         <v>37604561500</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="11">
         <f>I24/F24</f>
         <v>26434057.487100903</v>
       </c>
       <c r="K24" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L24" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L24" s="14">
         <f>K24*I24/1000</f>
-        <v>2.25627369</v>
+        <v>2.3434335426446999</v>
       </c>
       <c r="M24" t="s">
         <v>133</v>
       </c>
-      <c r="P24" t="s">
+      <c r="S24" t="s">
         <v>130</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="T24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:20">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="13"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>138</v>
       </c>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="K27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>20140508</v>
       </c>
@@ -4018,8 +4092,8 @@
         <v>30866</v>
       </c>
       <c r="F29" s="4">
-        <f>E29/100</f>
-        <v>308.66000000000003</v>
+        <f>E29/100-10</f>
+        <v>298.66000000000003</v>
       </c>
       <c r="G29">
         <v>11</v>
@@ -4027,20 +4101,21 @@
       <c r="H29" s="1">
         <v>78500</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="12">
         <f>H29*D29</f>
         <v>7961548500</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="16">
         <f>I29/F29</f>
-        <v>25793910.775610704</v>
+        <v>26657565.459050424</v>
       </c>
       <c r="K29" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L29" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L29" s="14">
         <f>K29*I29/1000</f>
-        <v>0.47769290999999997</v>
+        <v>0.4961461871133</v>
       </c>
       <c r="M29" t="s">
         <v>168</v>
@@ -4048,18 +4123,27 @@
       <c r="N29">
         <v>4</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
+        <v>10</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29" s="1">
         <f>N29/I29/2500</f>
         <v>2.0096593018305422E-13</v>
       </c>
-      <c r="P29" t="s">
+      <c r="S29" t="s">
         <v>144</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="T29" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>20140508</v>
       </c>
@@ -4076,8 +4160,8 @@
         <v>176528</v>
       </c>
       <c r="F30" s="4">
-        <f>E30/100</f>
-        <v>1765.28</v>
+        <f>E30/100-10</f>
+        <v>1755.28</v>
       </c>
       <c r="G30">
         <v>11</v>
@@ -4085,20 +4169,21 @@
       <c r="H30" s="1">
         <v>78500</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="12">
         <f>H30*D30</f>
         <v>46647133500</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="16">
         <f>I30/F30</f>
-        <v>26424778.788634099</v>
+        <v>26575323.310241103</v>
       </c>
       <c r="K30" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L30" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L30" s="14">
         <f>K30*I30/1000</f>
-        <v>2.7988280099999998</v>
+        <v>2.9069467360263004</v>
       </c>
       <c r="M30" t="s">
         <v>169</v>
@@ -4106,15 +4191,15 @@
       <c r="N30">
         <v>3</v>
       </c>
-      <c r="O30" s="1">
+      <c r="R30" s="1">
         <f>N30/I30/2500</f>
         <v>2.5725053394760047E-14</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="T30" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>20140508</v>
       </c>
@@ -4131,8 +4216,8 @@
         <v>85671</v>
       </c>
       <c r="F31" s="4">
-        <f>E31/100</f>
-        <v>856.71</v>
+        <f>E31/100-10</f>
+        <v>846.71</v>
       </c>
       <c r="G31">
         <v>11</v>
@@ -4140,20 +4225,21 @@
       <c r="H31" s="1">
         <v>78500</v>
       </c>
-      <c r="I31" s="13">
+      <c r="I31" s="12">
         <f>H31*D31</f>
         <v>82122539500</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="16">
         <f>I31/F31</f>
-        <v>95858037.725718156</v>
+        <v>96990161.330325603</v>
       </c>
       <c r="K31" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L31" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L31" s="14">
         <f>K31*I31/1000</f>
-        <v>4.9273523699999995</v>
+        <v>5.1176959920531004</v>
       </c>
       <c r="M31" t="s">
         <v>170</v>
@@ -4161,15 +4247,15 @@
       <c r="N31">
         <v>5</v>
       </c>
-      <c r="O31" s="1">
+      <c r="R31" s="1">
         <f>N31/I31/2500</f>
         <v>2.4353849895253177E-14</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>20140508</v>
       </c>
@@ -4186,8 +4272,8 @@
         <v>99494</v>
       </c>
       <c r="F32" s="4">
-        <f>E32/100</f>
-        <v>994.94</v>
+        <f>E32/100-10</f>
+        <v>984.94</v>
       </c>
       <c r="G32">
         <v>11</v>
@@ -4195,20 +4281,21 @@
       <c r="H32" s="1">
         <v>78500</v>
       </c>
-      <c r="I32" s="13">
+      <c r="I32" s="12">
         <f>H32*D32</f>
         <v>94304169500</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="16">
         <f>I32/F32</f>
-        <v>94783775.403541923</v>
+        <v>95746105.854163706</v>
       </c>
       <c r="K32" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L32" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L32" s="14">
         <f>K32*I32/1000</f>
-        <v>5.6582501699999996</v>
+        <v>5.8768283740671006</v>
       </c>
       <c r="M32" t="s">
         <v>171</v>
@@ -4216,27 +4303,42 @@
       <c r="N32">
         <v>5</v>
       </c>
-      <c r="O32" s="1">
+      <c r="R32" s="1">
         <f>N32/I32/2500</f>
         <v>2.1207970025121744E-14</v>
       </c>
-      <c r="P32" t="s">
+      <c r="S32" t="s">
         <v>143</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="T32" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="33" spans="1:20">
+      <c r="F33" s="4">
+        <f>SUM(F28:F32)</f>
+        <v>3885.59</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="14">
+        <f>SUM(L29:L32)</f>
+        <v>14.3976172892598</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" t="s">
         <v>139</v>
       </c>
       <c r="B34" t="s">
         <v>141</v>
       </c>
+      <c r="K34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="35" spans="1:20">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36">
         <v>20140508</v>
       </c>
@@ -4253,26 +4355,27 @@
         <v>8428</v>
       </c>
       <c r="F36" s="4">
-        <f>E36/100</f>
-        <v>84.28</v>
+        <f>E36/100-10</f>
+        <v>74.28</v>
       </c>
       <c r="H36" s="1">
         <v>78500</v>
       </c>
-      <c r="I36" s="13">
+      <c r="I36" s="12">
         <f>H36*D36</f>
         <v>6193257500</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="16">
         <f>I36/F36</f>
-        <v>73484308.258186996</v>
+        <v>83377187.668282181</v>
       </c>
       <c r="K36" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L36" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L36" s="14">
         <f>K36*I36/1000</f>
-        <v>0.37159544999999999</v>
+        <v>0.38595018223350003</v>
       </c>
       <c r="M36" t="s">
         <v>172</v>
@@ -4280,18 +4383,18 @@
       <c r="N36">
         <v>2</v>
       </c>
-      <c r="O36" s="1">
+      <c r="R36" s="1">
         <f>N36/I36/2500</f>
         <v>1.291727334121018E-13</v>
       </c>
-      <c r="P36" t="s">
+      <c r="S36" t="s">
         <v>140</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="T36" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:20">
       <c r="A37">
         <v>20140508</v>
       </c>
@@ -4308,26 +4411,27 @@
         <v>9290</v>
       </c>
       <c r="F37" s="4">
-        <f>E37/100</f>
-        <v>92.9</v>
+        <f>E37/100-10</f>
+        <v>82.9</v>
       </c>
       <c r="H37" s="1">
         <v>78500</v>
       </c>
-      <c r="I37" s="13">
+      <c r="I37" s="12">
         <f>H37*D37</f>
         <v>8072469000</v>
       </c>
-      <c r="J37" s="12">
+      <c r="J37" s="16">
         <f>I37/F37</f>
-        <v>86894176.533907428</v>
+        <v>97375983.112183347</v>
       </c>
       <c r="K37" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L37" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L37" s="14">
         <f>K37*I37/1000</f>
-        <v>0.48434813999999993</v>
+        <v>0.50305850864820001</v>
       </c>
       <c r="M37" t="s">
         <v>173</v>
@@ -4335,15 +4439,15 @@
       <c r="N37">
         <v>1</v>
       </c>
-      <c r="O37" s="1">
+      <c r="R37" s="1">
         <f>N37/I37/2500</f>
         <v>4.9551134851059822E-14</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="T37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:20">
       <c r="A38">
         <v>20140508</v>
       </c>
@@ -4360,26 +4464,27 @@
         <v>55897</v>
       </c>
       <c r="F38" s="4">
-        <f>E38/100</f>
-        <v>558.97</v>
+        <f>E38/100-10</f>
+        <v>548.97</v>
       </c>
       <c r="H38" s="1">
         <v>78500</v>
       </c>
-      <c r="I38" s="13">
+      <c r="I38" s="12">
         <f>H38*D38</f>
         <v>52721620500</v>
       </c>
-      <c r="J38" s="12">
+      <c r="J38" s="16">
         <f>I38/F38</f>
-        <v>94319230.906846523</v>
+        <v>96037343.570686921</v>
       </c>
       <c r="K38" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L38" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L38" s="14">
         <f>K38*I38/1000</f>
-        <v>3.1632972299999995</v>
+        <v>3.2854954019949005</v>
       </c>
       <c r="M38" t="s">
         <v>174</v>
@@ -4387,15 +4492,15 @@
       <c r="N38">
         <v>3</v>
       </c>
-      <c r="O38" s="1">
+      <c r="R38" s="1">
         <f>N38/I38/2500</f>
         <v>2.2761060616488446E-14</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="T38" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:20">
       <c r="A39">
         <v>20140508</v>
       </c>
@@ -4412,26 +4517,27 @@
         <v>238317</v>
       </c>
       <c r="F39" s="4">
-        <f>E39/100</f>
-        <v>2383.17</v>
+        <f>E39/100-10</f>
+        <v>2373.17</v>
       </c>
       <c r="H39" s="1">
         <v>78500</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="12">
         <f>H39*D39</f>
         <v>226185190000</v>
       </c>
-      <c r="J39" s="12">
+      <c r="J39" s="16">
         <f>I39/F39</f>
-        <v>94909381.202348128</v>
+        <v>95309307.803486466</v>
       </c>
       <c r="K39" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L39" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L39" s="14">
         <f>K39*I39/1000</f>
-        <v>13.571111399999998</v>
+        <v>14.095363433382001</v>
       </c>
       <c r="M39" t="s">
         <v>179</v>
@@ -4439,26 +4545,36 @@
       <c r="N39">
         <v>10</v>
       </c>
-      <c r="O39" s="1">
+      <c r="R39" s="1">
         <f>N39/I39/2500</f>
         <v>1.7684623825282283E-14</v>
       </c>
-      <c r="P39" t="s">
+      <c r="S39" t="s">
         <v>148</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="T39" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="1:17">
+    <row r="40" spans="1:20">
+      <c r="F40" s="4">
+        <f>SUM(F36:F39)</f>
+        <v>3079.32</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="14">
+        <f>SUM(L36:L39)</f>
+        <v>18.269867526258601</v>
+      </c>
+      <c r="R40" s="1"/>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42">
         <v>20140509</v>
       </c>
@@ -4484,20 +4600,21 @@
       <c r="H42" s="1">
         <v>78500</v>
       </c>
-      <c r="I42" s="13">
+      <c r="I42" s="12">
         <f>H42*D42</f>
         <v>125774505500</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="11">
         <f>I42/F42</f>
         <v>97862999.43199943</v>
       </c>
       <c r="K42" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L42" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L42" s="14">
         <f>K42*I42/1000</f>
-        <v>7.5464703299999991</v>
+        <v>7.8379904788479005</v>
       </c>
       <c r="M42" t="s">
         <v>175</v>
@@ -4505,18 +4622,18 @@
       <c r="N42">
         <v>6</v>
       </c>
-      <c r="O42" s="1">
+      <c r="R42" s="1">
         <f>N42/I42</f>
         <v>4.7704421306589835E-11</v>
       </c>
-      <c r="P42" t="s">
+      <c r="S42" t="s">
         <v>150</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="T42" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:20">
       <c r="A43">
         <v>20140509</v>
       </c>
@@ -4542,20 +4659,21 @@
       <c r="H43" s="1">
         <v>78500</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="12">
         <f>H43*D43</f>
         <v>32171498000</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J43" s="11">
         <f>I43/F43</f>
         <v>36668108.095786273</v>
       </c>
       <c r="K43" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L43" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L43" s="14">
         <f>K43*I43/1000</f>
-        <v>1.9302898799999999</v>
+        <v>2.0048569780644003</v>
       </c>
       <c r="M43" t="s">
         <v>176</v>
@@ -4563,15 +4681,15 @@
       <c r="N43">
         <v>5</v>
       </c>
-      <c r="O43" s="1">
+      <c r="R43" s="1">
         <f>N43/I43</f>
         <v>1.5541707134681761E-10</v>
       </c>
-      <c r="P43" t="s">
+      <c r="S43" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:20">
       <c r="A44">
         <v>20140509</v>
       </c>
@@ -4597,20 +4715,21 @@
       <c r="H44" s="1">
         <v>78500</v>
       </c>
-      <c r="I44" s="13">
+      <c r="I44" s="12">
         <f>H44*D44</f>
         <v>274847654000</v>
       </c>
-      <c r="J44" s="12">
+      <c r="J44" s="11">
         <f>I44/F44</f>
         <v>145626995.66585776</v>
       </c>
       <c r="K44" s="1">
-        <v>5.9999999999999995E-8</v>
-      </c>
-      <c r="L44" s="15">
+        <f>Sheet2!$C$12*Sheet2!$C$21</f>
+        <v>6.2317800000000005E-8</v>
+      </c>
+      <c r="L44" s="14">
         <f>K44*I44/1000</f>
-        <v>16.490859239999999</v>
+        <v>17.127901132441202</v>
       </c>
       <c r="M44" t="s">
         <v>177</v>
@@ -4618,50 +4737,50 @@
       <c r="N44">
         <v>23</v>
       </c>
-      <c r="O44" s="1">
+      <c r="R44" s="1">
         <f>N44/I44</f>
         <v>8.3682722647507119E-11</v>
       </c>
-      <c r="P44" t="s">
+      <c r="S44" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
-      <c r="O46" s="1"/>
-    </row>
-    <row r="48" spans="1:17">
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-    </row>
-    <row r="51" spans="1:23">
+    <row r="46" spans="1:20">
+      <c r="R46" s="1"/>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="51" spans="1:26">
       <c r="A51" t="s">
         <v>153</v>
       </c>
-      <c r="S51" t="s">
+      <c r="V51" t="s">
         <v>1</v>
       </c>
-      <c r="U51" t="s">
+      <c r="X51" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:26">
       <c r="N52" t="s">
         <v>155</v>
       </c>
-      <c r="O52" t="s">
+      <c r="R52" t="s">
         <v>156</v>
       </c>
-      <c r="P52" t="s">
+      <c r="S52" t="s">
         <v>157</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="T52" t="s">
         <v>158</v>
       </c>
-      <c r="R52" t="s">
+      <c r="U52" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:26">
       <c r="A53">
         <v>20140509</v>
       </c>
@@ -4687,18 +4806,18 @@
       <c r="H53" s="1">
         <v>78500</v>
       </c>
-      <c r="I53" s="13">
+      <c r="I53" s="12">
         <f>H53*D53</f>
         <v>4299602000</v>
       </c>
-      <c r="J53" s="12">
+      <c r="J53" s="11">
         <f>I53/F53</f>
         <v>23749458.683163941</v>
       </c>
       <c r="K53" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L53" s="15">
+      <c r="L53" s="14">
         <f>K53*I53/1000</f>
         <v>0.25797611999999998</v>
       </c>
@@ -4708,31 +4827,31 @@
       <c r="N53">
         <v>460</v>
       </c>
-      <c r="O53">
+      <c r="R53">
         <v>427</v>
       </c>
-      <c r="P53">
+      <c r="S53">
         <v>440</v>
       </c>
-      <c r="Q53">
+      <c r="T53">
         <v>454</v>
       </c>
-      <c r="R53">
+      <c r="U53">
         <v>1781</v>
       </c>
-      <c r="S53" s="1">
-        <f>R53/I53/U53</f>
+      <c r="V53" s="1">
+        <f>U53/I53/X53</f>
         <v>2.4689697405706551E-14</v>
       </c>
-      <c r="U53">
+      <c r="X53">
         <f>2^24</f>
         <v>16777216</v>
       </c>
-      <c r="W53" t="s">
+      <c r="Z53" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:26">
       <c r="A54">
         <v>20140509</v>
       </c>
@@ -4758,18 +4877,18 @@
       <c r="H54" s="1">
         <v>78500</v>
       </c>
-      <c r="I54" s="13">
+      <c r="I54" s="12">
         <f>H54*D54</f>
         <v>11429129000</v>
       </c>
-      <c r="J54" s="12">
+      <c r="J54" s="11">
         <f>I54/F54</f>
         <v>94776755.949912921</v>
       </c>
       <c r="K54" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L54" s="15">
+      <c r="L54" s="14">
         <f>K54*I54/1000</f>
         <v>0.68574773999999994</v>
       </c>
@@ -4779,31 +4898,31 @@
       <c r="N54">
         <v>1050</v>
       </c>
-      <c r="O54">
+      <c r="R54">
         <v>1120</v>
       </c>
-      <c r="P54">
+      <c r="S54">
         <v>1131</v>
       </c>
-      <c r="Q54">
+      <c r="T54">
         <v>1137</v>
       </c>
-      <c r="R54">
+      <c r="U54">
         <v>4438</v>
       </c>
-      <c r="S54" s="1">
-        <f>R54/I54/U54</f>
+      <c r="V54" s="1">
+        <f>U54/I54/X54</f>
         <v>2.3144844503302359E-14</v>
       </c>
-      <c r="U54">
+      <c r="X54">
         <f>2^24</f>
         <v>16777216</v>
       </c>
-      <c r="W54" t="s">
+      <c r="Z54" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:26">
       <c r="A55">
         <v>20140509</v>
       </c>
@@ -4829,18 +4948,18 @@
       <c r="H55" s="1">
         <v>78500</v>
       </c>
-      <c r="I55" s="13">
+      <c r="I55" s="12">
         <f>H55*D55</f>
         <v>5785999500</v>
       </c>
-      <c r="J55" s="12">
+      <c r="J55" s="11">
         <f>I55/F55</f>
         <v>94992603.841733709</v>
       </c>
       <c r="K55" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L55" s="15">
+      <c r="L55" s="14">
         <f>K55*I55/1000</f>
         <v>0.34715996999999998</v>
       </c>
@@ -4850,31 +4969,31 @@
       <c r="N55">
         <v>575</v>
       </c>
-      <c r="O55">
+      <c r="R55">
         <v>528</v>
       </c>
-      <c r="P55">
+      <c r="S55">
         <v>600</v>
       </c>
-      <c r="Q55">
+      <c r="T55">
         <v>547</v>
       </c>
-      <c r="R55">
+      <c r="U55">
         <v>2250</v>
       </c>
-      <c r="S55" s="1">
-        <f>R55/I55/U55</f>
+      <c r="V55" s="1">
+        <f>U55/I55/X55</f>
         <v>2.3178441468000282E-14</v>
       </c>
-      <c r="U55">
+      <c r="X55">
         <f>2^24</f>
         <v>16777216</v>
       </c>
-      <c r="W55" t="s">
+      <c r="Z55" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:26">
       <c r="A56">
         <v>20140509</v>
       </c>
@@ -4900,18 +5019,18 @@
       <c r="H56" s="1">
         <v>78500</v>
       </c>
-      <c r="I56" s="13">
+      <c r="I56" s="12">
         <f>H56*D56</f>
         <v>3609587000</v>
       </c>
-      <c r="J56" s="12">
+      <c r="J56" s="11">
         <f>I56/F56</f>
         <v>24012686.269292179</v>
       </c>
       <c r="K56" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L56" s="15">
+      <c r="L56" s="14">
         <f>K56*I56/1000</f>
         <v>0.21657521999999998</v>
       </c>
@@ -4921,36 +5040,36 @@
       <c r="N56">
         <v>327</v>
       </c>
-      <c r="O56">
+      <c r="R56">
         <v>365</v>
       </c>
-      <c r="P56">
+      <c r="S56">
         <v>334</v>
       </c>
-      <c r="Q56">
+      <c r="T56">
         <v>346</v>
       </c>
-      <c r="R56">
+      <c r="U56">
         <v>1372</v>
       </c>
-      <c r="S56" s="1">
-        <f>R56/I56/U56</f>
+      <c r="V56" s="1">
+        <f>U56/I56/X56</f>
         <v>2.2655659118850977E-14</v>
       </c>
-      <c r="U56">
+      <c r="X56">
         <f>2^24</f>
         <v>16777216</v>
       </c>
-      <c r="W56" t="s">
+      <c r="Z56" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:26">
       <c r="A59" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:26">
       <c r="A61">
         <v>20140509</v>
       </c>
@@ -4973,29 +5092,29 @@
       <c r="H61" s="1">
         <v>78500</v>
       </c>
-      <c r="I61" s="13">
+      <c r="I61" s="12">
         <f>H61*D61</f>
         <v>18538481500</v>
       </c>
-      <c r="J61" s="12">
+      <c r="J61" s="11">
         <f>I61/F61</f>
         <v>92659976.508222118</v>
       </c>
       <c r="K61" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L61" s="15">
+      <c r="L61" s="14">
         <f>K61*I61/1000</f>
         <v>1.1123088899999998</v>
       </c>
       <c r="M61" t="s">
         <v>178</v>
       </c>
-      <c r="P61" t="s">
+      <c r="S61" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:26">
       <c r="D62">
         <v>501203</v>
       </c>
@@ -5009,26 +5128,26 @@
       <c r="H62" s="1">
         <v>78500</v>
       </c>
-      <c r="I62" s="13">
+      <c r="I62" s="12">
         <f>H62*D62</f>
         <v>39344435500</v>
       </c>
-      <c r="J62" s="12" t="e">
+      <c r="J62" s="11" t="e">
         <f>I62/F62</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K62" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L62" s="15">
+      <c r="L62" s="14">
         <f>K62*I62/1000</f>
         <v>2.3606661299999998</v>
       </c>
-      <c r="P62" t="s">
+      <c r="S62" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:26">
       <c r="D63">
         <v>749227</v>
       </c>
@@ -5038,49 +5157,52 @@
       <c r="H63" s="1">
         <v>78500</v>
       </c>
-      <c r="I63" s="13">
+      <c r="I63" s="12">
         <f>H63*D63</f>
         <v>58814319500</v>
       </c>
-      <c r="J63" s="12" t="e">
+      <c r="J63" s="11" t="e">
         <f>I63/F63</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K63" s="1">
         <v>5.9999999999999995E-8</v>
       </c>
-      <c r="L63" s="15">
+      <c r="L63" s="14">
         <f>K63*I63/1000</f>
         <v>3.5288591699999996</v>
       </c>
-      <c r="P63" t="s">
+      <c r="S63" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
-      <c r="P64" t="s">
+    <row r="64" spans="1:26">
+      <c r="S64" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="2:15">
-      <c r="I65" s="13"/>
+    <row r="65" spans="2:18">
+      <c r="I65" s="12"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="13"/>
+      <c r="L65" s="12"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
-    </row>
-    <row r="69" spans="2:15">
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+    </row>
+    <row r="69" spans="2:18">
       <c r="B69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="72" spans="2:15">
+    <row r="72" spans="2:18">
       <c r="B72">
         <v>2</v>
       </c>
-      <c r="I72" s="13">
+      <c r="I72" s="12">
         <v>2E-14</v>
       </c>
       <c r="J72">
@@ -5089,7 +5211,7 @@
       <c r="K72" s="1">
         <v>100000000</v>
       </c>
-      <c r="L72" s="13">
+      <c r="L72" s="12">
         <f>K72*J72*I72</f>
         <v>0.02</v>
       </c>
@@ -5098,17 +5220,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="2:15">
+    <row r="73" spans="2:18">
       <c r="B73">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:15">
+    <row r="74" spans="2:18">
       <c r="B74">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:15">
+    <row r="75" spans="2:18">
       <c r="E75" t="s">
         <v>89</v>
       </c>
@@ -5121,11 +5243,11 @@
       <c r="H75" t="s">
         <v>92</v>
       </c>
-      <c r="I75" s="14" t="s">
+      <c r="I75" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="2:15">
+    <row r="76" spans="2:18">
       <c r="B76" s="1"/>
       <c r="E76">
         <v>19453</v>
@@ -5140,7 +5262,7 @@
         <f>1/G76</f>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="I76" s="14">
+      <c r="I76" s="13">
         <v>0.12</v>
       </c>
       <c r="J76" s="7">
@@ -5160,16 +5282,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:H23"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5205,7 +5327,7 @@
       <c r="C10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5217,11 +5339,42 @@
         <v>105</v>
       </c>
       <c r="C12" s="1">
-        <f>1.6E-19*1000000*100/(0.000001*1000)</f>
-        <v>1.6000000000000001E-8</v>
+        <f>1.602E-19*1000000*100/(0.000001*1000)</f>
+        <v>1.6020000000000001E-8</v>
       </c>
       <c r="D12" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" s="1">
+        <f>1/C12</f>
+        <v>62421972.534332082</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21">
+        <v>3.89</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23">
+        <f>10^-3</f>
+        <v>1E-3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>